<commit_message>
find first and last data cell
</commit_message>
<xml_diff>
--- a/resource/testData/part1.xlsx
+++ b/resource/testData/part1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0224B875-9EA5-44D2-BA48-F9EAD704CB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9DC762-B748-4110-A63B-B54C9DAB6EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{052D3BBF-3AE4-4211-8388-46A5DBAFB9C2}"/>
   </bookViews>
@@ -484,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95629AD8-A35F-4EE6-8A48-6ABCE163CA8D}">
-  <dimension ref="A3:D13"/>
+  <dimension ref="E13:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,157 +498,157 @@
     <col min="4" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E14">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F14" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G14" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E15">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G16" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F17" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G17" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E18">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F18" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="G18" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="F19" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
+      <c r="H19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E20">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="F20" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G20" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="H20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E21">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F21" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G21" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
+      <c r="H21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E22">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="F22" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G22" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="H22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E23">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F23" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G23" t="s">
         <v>24</v>
       </c>
-      <c r="D13" t="s">
+      <c r="H23" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>